<commit_message>
Changed the range of Grepseqs, from 150 to 20:90
</commit_message>
<xml_diff>
--- a/GREPore-seq_Template.us.xlsx
+++ b/GREPore-seq_Template.us.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="212" documentId="11_AD4DA82427541F7ACA7EB8C7F84D1CDE6BE8DE17" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A557570E-3AD9-4028-9C78-65F56F1B1853}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="4680" windowWidth="27930" windowHeight="15885" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2550" yWindow="3330" windowWidth="19065" windowHeight="12915" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RefInfo" sheetId="2" r:id="rId1"/>
@@ -1533,7 +1533,7 @@
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>